<commit_message>
Add beam waist distance column
</commit_message>
<xml_diff>
--- a/Python/HEL/data/Effectors.xlsx
+++ b/Python/HEL/data/Effectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Desktop\GITHUB_REPOSITORIES\Sandbox\Python\HEL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEE1EDE-1318-4430-8C08-7FFC424437D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C910287D-8A30-4D39-99DD-A60CC35A0754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E34359C3-189C-4E68-A285-9E32788085E5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Time (initial)</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>HEL2</t>
+  </si>
+  <si>
+    <t>r0</t>
   </si>
 </sst>
 </file>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05EF1A0-43A5-4589-AF84-11F2AD06417B}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,13 +453,14 @@
     <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -488,19 +492,22 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -531,20 +538,23 @@
       <c r="J2" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="K2" s="1">
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>0.5</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -575,16 +585,19 @@
       <c r="J3" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="K3">
-        <v>0</v>
+      <c r="K3" s="1">
+        <v>1000</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>0.5</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>

</xml_diff>